<commit_message>
reduce budget to see response
</commit_message>
<xml_diff>
--- a/betterhome-order-form.xlsx
+++ b/betterhome-order-form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narasimhan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narasimhan/workarea/betterhome/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9464964E-504F-CA48-B350-59F1886E51A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A51E2AD-5929-6C40-8CD7-176083693B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -250,6 +250,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -348,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -364,6 +371,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,9 +683,9 @@
   </sheetPr>
   <dimension ref="A1:AW2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="239" zoomScaleNormal="239" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="239" zoomScaleNormal="239" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -735,7 +745,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -900,7 +910,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="5">
-        <v>500000</v>
+        <v>200000</v>
       </c>
       <c r="I2" s="5">
         <v>3</v>

</xml_diff>